<commit_message>
feat: refactored code to specify variable types
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t xml:space="preserve">Employee ID</t>
   </si>
@@ -71,43 +71,52 @@
     <t xml:space="preserve">Phoo</t>
   </si>
   <si>
+    <t xml:space="preserve">Vailand at Gum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PigLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GumGum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gooo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LalaLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gul</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pepa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PigLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GumGum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gooo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LalaLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gul</t>
   </si>
 </sst>
 </file>
@@ -212,13 +221,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -330,6 +339,20 @@
         <v>21</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>8291</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -355,20 +378,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -385,7 +408,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1000</v>
@@ -419,7 +442,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>1234</v>
@@ -436,7 +459,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>1234</v>

</xml_diff>

<commit_message>
feat: added variables to count updated and inserted rows
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t xml:space="preserve">Employee ID</t>
   </si>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">Shyam</t>
   </si>
   <si>
-    <t xml:space="preserve">VaiLand</t>
+    <t xml:space="preserve">Vailand at Gum</t>
   </si>
   <si>
     <t xml:space="preserve">Mohul</t>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">Phoo</t>
   </si>
   <si>
-    <t xml:space="preserve">Vailand at Gum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pepa</t>
   </si>
   <si>
@@ -96,6 +93,15 @@
   </si>
   <si>
     <t xml:space="preserve">Tum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondLand</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -221,10 +227,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -308,7 +314,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>1234</v>
@@ -319,13 +325,13 @@
         <v>8912</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,13 +339,13 @@
         <v>1281</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,13 +353,27 @@
         <v>8291</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8273</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>22</v>
+      <c r="C9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -375,23 +395,23 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -408,7 +428,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1000</v>
@@ -442,7 +462,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>1234</v>
@@ -459,7 +479,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>1234</v>
@@ -470,13 +490,13 @@
         <v>8912</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>